<commit_message>
Implemented service-to-port mapping, fixed weak protocol detection (substring match), and applied numeric ID filtering so only real vendor rules are parsed.
</commit_message>
<xml_diff>
--- a/sample_data/CLIENT1 Firewall Rules - Anonymised - Firewall Policy-EXTERNAL-FW-DC - WITH RISK FEEDBACK.xlsx
+++ b/sample_data/CLIENT1 Firewall Rules - Anonymised - Firewall Policy-EXTERNAL-FW-DC - WITH RISK FEEDBACK.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\LTU Y3 Final Semester\Capstone Project\Projects\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\LTU Y3 Final Semester\Capstone Project\FireFind\sample_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{013FE211-51D2-488E-A4D1-B3852E7726C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E0711A9-B4F8-4777-B267-E57EB2A9BF53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" tabRatio="783" xr2:uid="{B6AE9014-F718-46DC-98F9-87914A7F25A7}"/>
   </bookViews>
@@ -795,8 +795,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A56C6DE-BDA8-4D92-8F57-0040D91A1C9A}">
   <dimension ref="A1:AI17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
-      <selection activeCell="N16" sqref="N16"/>
+    <sheetView tabSelected="1" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
+      <selection activeCell="J24" sqref="J24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" outlineLevelRow="1" x14ac:dyDescent="0.45"/>
@@ -1694,6 +1694,28 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_Flow_SignoffStatus xmlns="4ddb804d-af7f-41e1-889b-2ef1cbcc2ac7" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="4ddb804d-af7f-41e1-889b-2ef1cbcc2ac7">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="d4c29202-6161-454f-9c20-780b5f768c27" xsi:nil="true"/>
+    <Createdby xmlns="4ddb804d-af7f-41e1-889b-2ef1cbcc2ac7" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010021A5C088B25E174C8D0227473E0E693C" ma:contentTypeVersion="29" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="3cc59f655b5269486b8b27279db258df">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="4ddb804d-af7f-41e1-889b-2ef1cbcc2ac7" xmlns:ns3="d4c29202-6161-454f-9c20-780b5f768c27" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="2b84ca775960dfd5d5582380a4ab113f" ns2:_="" ns3:_="">
     <xsd:import namespace="4ddb804d-af7f-41e1-889b-2ef1cbcc2ac7"/>
@@ -1966,43 +1988,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_Flow_SignoffStatus xmlns="4ddb804d-af7f-41e1-889b-2ef1cbcc2ac7" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="4ddb804d-af7f-41e1-889b-2ef1cbcc2ac7">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="d4c29202-6161-454f-9c20-780b5f768c27" xsi:nil="true"/>
-    <Createdby xmlns="4ddb804d-af7f-41e1-889b-2ef1cbcc2ac7" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8AD3E354-DDB1-4931-B7C1-B152100CE749}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9B1B530A-5435-4A38-97B9-3507A1AB69AC}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="4ddb804d-af7f-41e1-889b-2ef1cbcc2ac7"/>
-    <ds:schemaRef ds:uri="d4c29202-6161-454f-9c20-780b5f768c27"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2025,9 +2014,20 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9B1B530A-5435-4A38-97B9-3507A1AB69AC}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8AD3E354-DDB1-4931-B7C1-B152100CE749}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="4ddb804d-af7f-41e1-889b-2ef1cbcc2ac7"/>
+    <ds:schemaRef ds:uri="d4c29202-6161-454f-9c20-780b5f768c27"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>